<commit_message>
updated the files for duplicate id bug fix, improved commandline usage
</commit_message>
<xml_diff>
--- a/test_resource/golden_Testcases_Duplicate_ID.xlsx
+++ b/test_resource/golden_Testcases_Duplicate_ID.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PythonRepo\TextSimilarityProcessor\test_resource\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Duplicate_ID" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -22,8 +27,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +91,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -132,7 +145,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,9 +177,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,6 +212,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -373,49 +388,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>101</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>101</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>